<commit_message>
Fixed SplashDialog. Working on Combat Calander.
</commit_message>
<xml_diff>
--- a/DesignDocs/Tables.xlsx
+++ b/DesignDocs/Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0E0B0759-06F6-46FF-8C32-57A24B458300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F9B7197-2814-4F00-8B69-13400632FBAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25974" yWindow="-109" windowWidth="26301" windowHeight="14889" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -34,307 +34,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>t226</t>
-  </si>
-  <si>
-    <t>t220</t>
-  </si>
-  <si>
-    <t>&lt;Table CellSpacing="2" BorderBrush="Black" BorderThickness="3"&gt;
-	&lt;TableRowGroup FontStyle="Italic" Background="Black" Foreground="White"&gt;
-		&lt;TableRow FontSize="12"&gt; 
-			&lt;TableCell  ColumnSpan="2" TextAlignment="Left"&gt;&lt;Paragraph&gt;&lt;Bold&gt;Result = striker skill - target skill - dice roll + modifiers&lt;/Bold&gt;&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt;
-		&lt;TableRow FontSize="12"&gt; 
-			&lt;TableCell  ColumnSpan="2" TextAlignment="Left"&gt;&lt;Paragraph&gt;&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt;
-		&lt;TableRow FontSize="12"&gt; 
-			&lt;TableCell  ColumnSpan="2" TextAlignment="Left"&gt;&lt;Paragraph TextDecorations='Underline'&gt;Modifiers:&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt;
-		&lt;TableRow FontSize="12"&gt; 
-			&lt;TableCell  ColumnSpan="2" TextAlignment="Left"&gt;&lt;Paragraph&gt;+2 target has wounds of one-half or more endurance&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt;
-		&lt;TableRow FontSize="12"&gt; 
-			&lt;TableCell  ColumnSpan="2" TextAlignment="Left"&gt;&lt;Paragraph&gt;-1 striker has one or more wound&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt;
-		&lt;TableRow FontSize="12"&gt; 
-			&lt;TableCell  ColumnSpan="2" TextAlignment="Left"&gt;&lt;Paragraph&gt;-1 striker has wounds of one-half or more his endurance&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt;
-		&lt;TableRow FontSize="12"&gt; 
-			&lt;TableCell  ColumnSpan="2" TextAlignment="Left"&gt;&lt;Paragraph&gt;-1 for each striker stavation day&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt;
-		&lt;TableRow FontSize="12"&gt; 
-			&lt;TableCell  ColumnSpan="2" TextAlignment="Left"&gt;&lt;Paragraph&gt;+1 for each target starvation day&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt;
-		&lt;TableRow FontSize="12"&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt;
-		&lt;TableRow FontSize="12"&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;Roll&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;# of wounds&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt;
-	&lt;/TableRowGroup&gt;
-	&lt;TableRowGroup&gt;
-		&lt;TableRow FontSize="12" FontFamily='Courier New'&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;-1&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;one&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt; 
-		&lt;TableRow FontSize="12" FontFamily='Courier New'&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;1&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;one&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt;
-		&lt;TableRow FontSize="12" FontFamily='Courier New'&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;3&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;one&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt;
-		&lt;TableRow FontSize="12" FontFamily='Courier New'&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;5&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;one&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt;
-		&lt;TableRow FontSize="12" FontFamily='Courier New'&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;8&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;one&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt;
-		&lt;TableRow FontSize="12" FontFamily='Courier New'&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;10&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;two&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt;
-		&lt;TableRow FontSize="12" FontFamily='Courier New'&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;11&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;one&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt;
-		&lt;TableRow FontSize="12" FontFamily='Courier New'&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;12&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;two&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt;
-		&lt;TableRow FontSize="12" FontFamily='Courier New'&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;13&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;two&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt;
-		&lt;TableRow FontSize="12" FontFamily='Courier New'&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;14&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;three&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt;
-		&lt;TableRow FontSize="12" FontFamily='Courier New'&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;16&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;five&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt;
-		&lt;TableRow FontSize="12" FontFamily='Courier New'&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;17&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;two&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt;
-		&lt;TableRow FontSize="12" FontFamily='Courier New'&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;18&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;five&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt;
-		&lt;TableRow FontSize="12" FontFamily='Courier New'&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;19&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;five&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt;
-		&lt;TableRow FontSize="12" FontFamily='Courier New'&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;20+&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;six&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt;
-	&lt;/TableRowGroup&gt;
-&lt;/Table&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Table CellSpacing="2" BorderBrush="Black" BorderThickness="3"&gt;
-	&lt;TableRowGroup FontStyle="Italic" Background="Black" Foreground="White"&gt;
-		&lt;TableRow FontSize="12"&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;Wealth Code&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;1&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;2&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;3&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;4&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;5&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;6&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt;
-	&lt;/TableRowGroup&gt;
-	&lt;TableRowGroup&gt;
-		&lt;TableRow FontSize="12" FontFamily='Courier New'&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;1&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;0&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;0&lt;/Paragraph&gt;&lt;/TableCell&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;1&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;1&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;2&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;2&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt; 
-		&lt;TableRow FontSize="12" FontFamily='Courier New'&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;2&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;0&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;1&lt;/Paragraph&gt;&lt;/TableCell&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;2&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;2&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;3&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;4&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt; 
-		&lt;TableRow FontSize="12" FontFamily='Courier New'&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;4&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;2&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;3&lt;/Paragraph&gt;&lt;/TableCell&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;4&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;4&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;5&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;6&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt; 
-		&lt;TableRow FontSize="12" FontFamily='Courier New'&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;5&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;2&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;3+A&lt;/Paragraph&gt;&lt;/TableCell&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;4&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;6+A&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;7&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;8+A&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt;
-		&lt;TableRow FontSize="12" FontFamily='Courier New'&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;7&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;3&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;4&lt;/Paragraph&gt;&lt;/TableCell&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;5&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;8&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;10&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;11&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt;
-		&lt;TableRow FontSize="12" FontFamily='Courier New'&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;10&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;6&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;8&lt;/Paragraph&gt;&lt;/TableCell&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;9&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;11&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;12&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;14&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt;
-		&lt;TableRow FontSize="12" FontFamily='Courier New'&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;12&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;5&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;9+C&lt;/Paragraph&gt;&lt;/TableCell&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;11+A&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;12&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;15+A&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;20&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt;
-		&lt;TableRow FontSize="12" FontFamily='Courier New'&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;15&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;10&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;12&lt;/Paragraph&gt;&lt;/TableCell&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;14&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;16&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;18&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;20&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt;
-		&lt;TableRow FontSize="12" FontFamily='Courier New'&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;21&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;15&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;18&lt;/Paragraph&gt;&lt;/TableCell&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;20&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;22&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;24&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;27&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt;
-		&lt;TableRow FontSize="12" FontFamily='Courier New'&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;25&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;20+A&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;22&lt;/Paragraph&gt;&lt;/TableCell&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;24+A&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;26&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;28+A&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;30&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt;
-		&lt;TableRow FontSize="12" FontFamily='Courier New'&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;30&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;23&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;27&lt;/Paragraph&gt;&lt;/TableCell&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;29&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;31&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;33&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;37&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt;
-		&lt;TableRow FontSize="12" FontFamily='Courier New'&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;50&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;40&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;45&lt;/Paragraph&gt;&lt;/TableCell&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;48&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;52&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;55&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;60&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt;
-		&lt;TableRow FontSize="12" FontFamily='Courier New'&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;60&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;45+A&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;50+C&lt;/Paragraph&gt;&lt;/TableCell&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;55&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;60+B&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;70+A&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;80&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt;
-		&lt;TableRow FontSize="12" FontFamily='Courier New'&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;70&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;55&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;60&lt;/Paragraph&gt;&lt;/TableCell&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;65&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;70&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;80&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;90&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt;
-		&lt;TableRow FontSize="12" FontFamily='Courier New'&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;100&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;85&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;90&lt;/Paragraph&gt;&lt;/TableCell&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;95&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;100&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;110&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;120&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt;
-		&lt;TableRow FontSize="12" FontFamily='Courier New'&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;110&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;80+B&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;90+C&lt;/Paragraph&gt;&lt;/TableCell&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;100+B&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;110+A&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;130+C&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;150+A&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt;
-		&lt;TableRow FontSize="12" FontFamily='Courier New'&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;A&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;&lt;InlineUIContainer&gt;&lt;Button Content='r180' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;&lt;InlineUIContainer&gt;&lt;Button Content='r181' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;&lt;InlineUIContainer&gt;&lt;Button Content='r182' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;&lt;InlineUIContainer&gt;&lt;Button Content='r183' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;&lt;InlineUIContainer&gt;&lt;Button Content='r184' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;&lt;InlineUIContainer&gt;&lt;Button Content='r185' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt;
-		&lt;TableRow FontSize="12" FontFamily='Courier New'&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;B&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;&lt;InlineUIContainer&gt;&lt;Button Content='r180' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;&lt;InlineUIContainer&gt;&lt;Button Content='r186' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;&lt;InlineUIContainer&gt;&lt;Button Content='r187' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;&lt;InlineUIContainer&gt;&lt;Button Content='r188' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;&lt;InlineUIContainer&gt;&lt;Button Content='r190' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;&lt;InlineUIContainer&gt;&lt;Button Content='r193' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt;
-		&lt;TableRow FontSize="12" FontFamily='Courier New'&gt;
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;C&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;&lt;InlineUIContainer&gt;&lt;Button Content='r186' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;&lt;InlineUIContainer&gt;&lt;Button Content='r188' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;&lt;InlineUIContainer&gt;&lt;Button Content='r189' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;&lt;InlineUIContainer&gt;&lt;Button Content='r191' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;&lt;InlineUIContainer&gt;&lt;Button Content='r192' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-			&lt;TableCell TextAlignment="Center"&gt;&lt;Paragraph&gt;&lt;InlineUIContainer&gt;&lt;Button Content='r194' FontFamily='Courier New' FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-		&lt;/TableRow&gt;
-	&lt;/TableRowGroup&gt;
-&lt;/Table&gt;</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>t001</t>
   </si>
   <si>
-    <t>&lt;Table CellSpacing="2" BorderBrush="Black" BorderThickness="3"&gt;
-&lt;Table.Columns&gt;&lt;TableColumn Width="*"/&gt;&lt;TableColumn Width="*"/&gt;&lt;TableColumn Width="3*"/&gt;&lt;/Table.Columns&gt;
+    <t>&lt;Table&gt;
 &lt;TableRowGroup  Name="myTableRowGroupHdr1" FontStyle="Italic" Background="Black" Foreground="White"&gt;
    &lt;TableRow Name="myTableRowHdr2" FontSize="12"&gt; 
       &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;Month&lt;LineBreak/&gt;Day&lt;/Paragraph&gt;&lt;/TableCell&gt; 
@@ -342,7 +47,7 @@
       &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;Historical Notes&lt;/Paragraph&gt;&lt;/TableCell&gt; 
    &lt;/TableRow&gt;
 &lt;/TableRowGroup&gt;
-&lt;TableRowGroup&gt;
+&lt;TableRowGroup Background="AliceBlue" &gt;
    &lt;TableRow FontSize="12"&gt;
       &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;7/27&lt;/Paragraph&gt;&lt;/TableCell&gt; 
       &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-3-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
@@ -350,24 +55,180 @@
    &lt;/TableRow&gt;
    &lt;TableRow FontSize="12"&gt;
       &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;7/28&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-3-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;B-4-M&lt;/Paragraph&gt;&lt;/TableCell&gt; 
       &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt;Coutances&lt;/Paragraph&gt;&lt;/TableCell&gt; 
    &lt;/TableRow&gt;
    &lt;TableRow FontSize="12"&gt;
       &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;7/29&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-3-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+   &lt;/TableRow&gt;
+   &lt;TableRow FontSize="12"&gt;
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;7/30&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-4-M&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell&gt; &lt;Paragraph&gt;Avranches&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+   &lt;/TableRow&gt;
+   &lt;TableRow FontSize="12"&gt;
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;7/31&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
       &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
    &lt;/TableRow&gt;
 &lt;/TableRowGroup&gt;
-&lt;TableRowGroup&gt;
-   &lt;TableRow FontSize="12"&gt;
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;7/30&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-3-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell  RowSpan="2" Padding="10"&gt; &lt;Paragraph&gt;Avranches&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-   &lt;/TableRow&gt;
-   &lt;TableRow FontSize="12"&gt;
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;7/31&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-3-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+&lt;TableRowGroup Background="LightGray" &gt;
+   &lt;TableRow FontSize="12"&gt;
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/01&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+   &lt;/TableRow&gt;
+   &lt;TableRow FontSize="12"&gt;
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/02&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+   &lt;/TableRow&gt;
+   &lt;TableRow FontSize="12"&gt;
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/03&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+   &lt;/TableRow&gt;
+   &lt;TableRow FontSize="12"&gt;
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/04&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+   &lt;/TableRow&gt;
+   &lt;TableRow FontSize="12"&gt;
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/05&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-4-H&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt;Vannes&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+   &lt;/TableRow&gt;
+   &lt;TableRow FontSize="12"&gt;
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/06&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+   &lt;/TableRow&gt;
+   &lt;TableRow FontSize="12"&gt;
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/07&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-4-H&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt;Lorient&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+   &lt;/TableRow&gt;
+   &lt;TableRow FontSize="12"&gt;
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/08&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+   &lt;/TableRow&gt;
+   &lt;TableRow FontSize="12"&gt;
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/09&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+   &lt;/TableRow&gt;
+   &lt;TableRow FontSize="12"&gt;
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/10&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+   &lt;/TableRow&gt;
+   &lt;TableRow FontSize="12"&gt;
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/11&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-4-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt;Nantes&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+   &lt;/TableRow&gt;
+   &lt;TableRow FontSize="12"&gt;
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/12&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+   &lt;/TableRow&gt;
+   &lt;TableRow FontSize="12"&gt;
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/13&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+   &lt;/TableRow&gt;
+   &lt;TableRow FontSize="12"&gt;
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/14&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+   &lt;/TableRow&gt;
+   &lt;TableRow FontSize="12"&gt;
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/15&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+   &lt;/TableRow&gt;
+   &lt;TableRow FontSize="12"&gt;
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/16&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-3-M&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt;Orleans&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+   &lt;/TableRow&gt;
+   &lt;TableRow FontSize="12"&gt;
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/17&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+   &lt;/TableRow&gt;
+   &lt;TableRow FontSize="12"&gt;
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/18&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+   &lt;/TableRow&gt;
+   &lt;TableRow FontSize="12"&gt;
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/19&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+   &lt;/TableRow&gt;
+   &lt;TableRow FontSize="12"&gt;
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/20&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+   &lt;/TableRow&gt;
+   &lt;TableRow FontSize="12"&gt;
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/21&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+   &lt;/TableRow&gt;
+   &lt;TableRow FontSize="12"&gt;
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/22&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+   &lt;/TableRow&gt;
+   &lt;TableRow FontSize="12"&gt;
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/23&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+   &lt;/TableRow&gt;
+   &lt;TableRow FontSize="12"&gt;
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/24&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+   &lt;/TableRow&gt;
+   &lt;TableRow FontSize="12"&gt;
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/25&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+   &lt;/TableRow&gt;
+   &lt;TableRow FontSize="12"&gt;
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/26&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+   &lt;/TableRow&gt;
+   &lt;TableRow FontSize="12"&gt;
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/27&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+   &lt;/TableRow&gt;
+   &lt;TableRow FontSize="12"&gt;
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/28&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+   &lt;/TableRow&gt;
+   &lt;TableRow FontSize="12"&gt;
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/29&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+   &lt;/TableRow&gt;
+   &lt;TableRow FontSize="12"&gt;
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/30&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+   &lt;/TableRow&gt;
+   &lt;TableRow FontSize="12"&gt;
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/31&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-4-M&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
    &lt;/TableRow&gt;
 &lt;/TableRowGroup&gt;
 &lt;/Table&gt;</t>
@@ -747,7 +608,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -760,32 +621,19 @@
   <sheetData>
     <row r="1" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>3</v>
-      </c>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B2" s="4"/>
     </row>
     <row r="65" ht="154.55000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B65">
-    <sortCondition ref="A2:A65"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B64">
+    <sortCondition ref="A2:A64"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished showing Combat Calander Table
</commit_message>
<xml_diff>
--- a/DesignDocs/Tables.xlsx
+++ b/DesignDocs/Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F9B7197-2814-4F00-8B69-13400632FBAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D8A58B6D-46C3-4D2D-937A-4546DA32F943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25974" yWindow="-109" windowWidth="26301" windowHeight="14889" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -39,199 +39,600 @@
     <t>t001</t>
   </si>
   <si>
-    <t>&lt;Table&gt;
-&lt;TableRowGroup  Name="myTableRowGroupHdr1" FontStyle="Italic" Background="Black" Foreground="White"&gt;
-   &lt;TableRow Name="myTableRowHdr2" FontSize="12"&gt; 
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;Month&lt;LineBreak/&gt;Day&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;Situation&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;Historical Notes&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-   &lt;/TableRow&gt;
-&lt;/TableRowGroup&gt;
-&lt;TableRowGroup Background="AliceBlue" &gt;
-   &lt;TableRow FontSize="12"&gt;
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;7/27&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-3-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt;Cobra Breakout&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-   &lt;/TableRow&gt;
-   &lt;TableRow FontSize="12"&gt;
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;7/28&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;B-4-M&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt;Coutances&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-   &lt;/TableRow&gt;
-   &lt;TableRow FontSize="12"&gt;
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;7/29&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
-   &lt;/TableRow&gt;
-   &lt;TableRow FontSize="12"&gt;
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;7/30&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-4-M&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell&gt; &lt;Paragraph&gt;Avranches&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-   &lt;/TableRow&gt;
-   &lt;TableRow FontSize="12"&gt;
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;7/31&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
-   &lt;/TableRow&gt;
-&lt;/TableRowGroup&gt;
-&lt;TableRowGroup Background="LightGray" &gt;
-   &lt;TableRow FontSize="12"&gt;
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/01&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
-   &lt;/TableRow&gt;
-   &lt;TableRow FontSize="12"&gt;
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/02&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
-   &lt;/TableRow&gt;
-   &lt;TableRow FontSize="12"&gt;
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/03&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
-   &lt;/TableRow&gt;
-   &lt;TableRow FontSize="12"&gt;
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/04&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
-   &lt;/TableRow&gt;
-   &lt;TableRow FontSize="12"&gt;
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/05&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-4-H&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt;Vannes&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-   &lt;/TableRow&gt;
-   &lt;TableRow FontSize="12"&gt;
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/06&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
-   &lt;/TableRow&gt;
-   &lt;TableRow FontSize="12"&gt;
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/07&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-4-H&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt;Lorient&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-   &lt;/TableRow&gt;
-   &lt;TableRow FontSize="12"&gt;
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/08&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
-   &lt;/TableRow&gt;
-   &lt;TableRow FontSize="12"&gt;
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/09&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
-   &lt;/TableRow&gt;
-   &lt;TableRow FontSize="12"&gt;
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/10&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
-   &lt;/TableRow&gt;
-   &lt;TableRow FontSize="12"&gt;
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/11&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-4-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt;Nantes&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-   &lt;/TableRow&gt;
-   &lt;TableRow FontSize="12"&gt;
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/12&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
-   &lt;/TableRow&gt;
-   &lt;TableRow FontSize="12"&gt;
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/13&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
-   &lt;/TableRow&gt;
-   &lt;TableRow FontSize="12"&gt;
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/14&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
-   &lt;/TableRow&gt;
-   &lt;TableRow FontSize="12"&gt;
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/15&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
-   &lt;/TableRow&gt;
-   &lt;TableRow FontSize="12"&gt;
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/16&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-3-M&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt;Orleans&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-   &lt;/TableRow&gt;
-   &lt;TableRow FontSize="12"&gt;
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/17&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
-   &lt;/TableRow&gt;
-   &lt;TableRow FontSize="12"&gt;
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/18&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
-   &lt;/TableRow&gt;
-   &lt;TableRow FontSize="12"&gt;
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/19&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
-   &lt;/TableRow&gt;
-   &lt;TableRow FontSize="12"&gt;
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/20&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
-   &lt;/TableRow&gt;
-   &lt;TableRow FontSize="12"&gt;
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/21&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
-   &lt;/TableRow&gt;
-   &lt;TableRow FontSize="12"&gt;
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/22&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
-   &lt;/TableRow&gt;
-   &lt;TableRow FontSize="12"&gt;
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/23&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
-   &lt;/TableRow&gt;
-   &lt;TableRow FontSize="12"&gt;
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/24&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
-   &lt;/TableRow&gt;
-   &lt;TableRow FontSize="12"&gt;
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/25&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
-   &lt;/TableRow&gt;
-   &lt;TableRow FontSize="12"&gt;
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/26&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
-   &lt;/TableRow&gt;
-   &lt;TableRow FontSize="12"&gt;
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/27&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
-   &lt;/TableRow&gt;
-   &lt;TableRow FontSize="12"&gt;
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/28&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
-   &lt;/TableRow&gt;
-   &lt;TableRow FontSize="12"&gt;
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/29&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
-   &lt;/TableRow&gt;
-   &lt;TableRow FontSize="12"&gt;
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/30&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
-   &lt;/TableRow&gt;
-   &lt;TableRow FontSize="12"&gt;
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/31&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-4-M&lt;/Paragraph&gt;&lt;/TableCell&gt; 
-      &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
-   &lt;/TableRow&gt;
-&lt;/TableRowGroup&gt;
-&lt;/Table&gt;</t>
+    <t xml:space="preserve">&lt;Table&gt;
+&lt;Table.Columns&gt;
+   &lt;TableColumn Width="300"/&gt;
+   &lt;TableColumn Width="300"/&gt;
+   &lt;TableColumn Width="300"/&gt;  
+   &lt;TableColumn Width="300"/&gt;  
+&lt;/Table.Columns&gt; 
+&lt;TableRowGroup  FontStyle="Italic" &gt;
+   &lt;TableRow FontSize="12"&gt; 
+      &lt;TableCell TextAlignment="Center"&gt;
+	  &lt;Table&gt;
+		&lt;Table.Columns&gt;
+		   &lt;TableColumn Width="50"/&gt;
+		   &lt;TableColumn Width="50"/&gt;
+		   &lt;TableColumn Width="180"/&gt;  
+		&lt;/Table.Columns&gt;   
+		&lt;TableRowGroup  FontStyle="Italic" Background="Black" Foreground="White"&gt;
+		   &lt;TableRow  FontSize="12"&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;Month&lt;LineBreak/&gt;Day&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;Situation&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;Historical Notes&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		&lt;/TableRowGroup&gt;
+		&lt;TableRowGroup Background="AliceBlue" &gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;7/27&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-3-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt;Cobra Breakout&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;7/28&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;B-4-M&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt;Coutances&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;7/29&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;7/30&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-4-M&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell&gt; &lt;Paragraph&gt;Avranches&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;7/31&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		&lt;/TableRowGroup&gt;
+		&lt;TableRowGroup Background="LightGray" &gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/01&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/02&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/03&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/04&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/05&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-4-H&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt;Vannes&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/06&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/07&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-4-H&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt;Lorient&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/08&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/09&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/10&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/11&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-4-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt;Nantes&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/12&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/13&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/14&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/15&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/16&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-3-M&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt;Orleans&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/17&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/18&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/19&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/20&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/21&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/22&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/23&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/24&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/25&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/26&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/27&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/28&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/29&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/30&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/31&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-4-M&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt;Commercy&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		&lt;/TableRowGroup&gt;
+		&lt;TableRowGroup Background="AliceBlue" &gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;9/01&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt;&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell ColumnSpan="3" TextAlignment="Center"&gt; &lt;Paragraph&gt;==========Refitting==========&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;9/11&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-5-H&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell RowSpan="3" TextAlignment="Left" BorderBrush="Black" BorderThickness="1"&gt; &lt;Paragraph&gt;&lt;LineBreak/&gt;Moselle Crossing&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;9/12&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;C-5-M&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;9/13&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;C-5-M&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;9/14&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-3-M&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt;Crevic and Maixe&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;9/15&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;B-9-M&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt;Luneville&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;   
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;9/16&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;B-9-M&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt; 
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;9/17&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-3-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt; 
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;9/18&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-3-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt; 
+			&lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;9/19&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;B-9-M&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell RowSpan="4" TextAlignment="Left" BorderBrush="Black" BorderThickness="1"&gt; &lt;Paragraph&gt;&lt;LineBreak/&gt;&lt;LineBreak/&gt;Arracourt&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt; 
+			&lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;9/20&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-3-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt; 
+			&lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;9/21&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;B-9-M&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt; 
+			&lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;9/22&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;B-9-M&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt; 
+			&lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell ColumnSpan="3" TextAlignment="Center"&gt; &lt;Paragraph&gt;==========Refitting==========&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;    
+		&lt;/TableRowGroup&gt;
+		&lt;/Table&gt;
+	  &lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Center"&gt;
+	  &lt;Table&gt;
+		&lt;Table.Columns&gt;
+		   &lt;TableColumn Width="50"/&gt;
+		   &lt;TableColumn Width="50"/&gt;
+		   &lt;TableColumn Width="180"/&gt;  
+		&lt;/Table.Columns&gt;   
+		&lt;TableRowGroup  FontStyle="Italic" Background="Black" Foreground="White"&gt;
+		   &lt;TableRow  FontSize="12"&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;Month&lt;LineBreak/&gt;Day&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;Situation&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;Historical Notes&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		&lt;/TableRowGroup&gt;
+		&lt;TableRowGroup Background="AliceBlue" &gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;7/27&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-3-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt;Cobra Breakout&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;7/28&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;B-4-M&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt;Coutances&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;7/29&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;7/30&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-4-M&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell&gt; &lt;Paragraph&gt;Avranches&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;7/31&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		&lt;/TableRowGroup&gt;
+		&lt;TableRowGroup Background="LightGray" &gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/01&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/02&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/03&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/04&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/05&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-4-H&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt;Vannes&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/06&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/07&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-4-H&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt;Lorient&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/08&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/09&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/10&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/11&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-4-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt;Nantes&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/12&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/13&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/14&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/15&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/16&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-3-M&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt;Orleans&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/17&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/18&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/19&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/20&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/21&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/22&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/23&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/24&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/25&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/26&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/27&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/28&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/29&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/30&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/31&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-4-M&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt;Commercy&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		&lt;/TableRowGroup&gt;
+		&lt;TableRowGroup Background="AliceBlue" &gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;9/01&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt;&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell ColumnSpan="3" TextAlignment="Center"&gt; &lt;Paragraph&gt;==========Refitting==========&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;9/11&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-5-H&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell RowSpan="3" TextAlignment="Left" BorderBrush="Black" BorderThickness="1"&gt; &lt;Paragraph&gt;&lt;LineBreak/&gt;Moselle Crossing&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;9/12&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;C-5-M&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;9/13&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;C-5-M&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;9/14&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-3-M&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt;Crevic and Maixe&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;9/15&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;B-9-M&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt;Luneville&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;   
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;9/16&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;B-9-M&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt; 
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;9/17&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-3-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt; 
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;9/18&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-3-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt; 
+			&lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;9/19&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;B-9-M&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell RowSpan="4" TextAlignment="Left" BorderBrush="Black" BorderThickness="1"&gt; &lt;Paragraph&gt;&lt;LineBreak/&gt;&lt;LineBreak/&gt;Arracourt&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt; 
+			&lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;9/20&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-3-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt; 
+			&lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;9/21&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;B-9-M&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt; 
+			&lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;9/22&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;B-9-M&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt; 
+			&lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell ColumnSpan="3" TextAlignment="Center"&gt; &lt;Paragraph&gt;==========Refitting==========&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;    
+		&lt;/TableRowGroup&gt;
+		&lt;/Table&gt;
+	  &lt;/TableCell&gt; 
+      &lt;TableCell TextAlignment="Center"&gt;
+	  &lt;Table&gt;
+		&lt;Table.Columns&gt;
+		   &lt;TableColumn Width="50"/&gt;
+		   &lt;TableColumn Width="50"/&gt;
+		   &lt;TableColumn Width="180"/&gt;  
+		&lt;/Table.Columns&gt;   
+		&lt;TableRowGroup  FontStyle="Italic" Background="Black" Foreground="White"&gt;
+		   &lt;TableRow  FontSize="12"&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;Month&lt;LineBreak/&gt;Day&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;Situation&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;Historical Notes&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		&lt;/TableRowGroup&gt;
+		&lt;TableRowGroup Background="AliceBlue" &gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;7/27&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-3-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt;Cobra Breakout&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;7/28&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;B-4-M&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt;Coutances&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;7/29&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;7/30&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-4-M&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell&gt; &lt;Paragraph&gt;Avranches&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;7/31&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		&lt;/TableRowGroup&gt;
+		&lt;TableRowGroup Background="LightGray" &gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;8/01&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Center"&gt; &lt;Paragraph&gt;A-2-L&lt;/Paragraph&gt;&lt;/TableCell&gt; 
+			  &lt;TableCell TextAlignment="Left"&gt; &lt;Paragraph&gt; &lt;/Paragraph&gt;&lt;/TableCell&gt; 
+		   &lt;/TableRow&gt;
+		   &lt;TableRow FontSize="12"&gt;
+			  &lt;TableCell TextAlignment="Center"&gt; </t>
   </si>
 </sst>
 </file>

</xml_diff>